<commit_message>
billing 2023_07 + huhtamaki
</commit_message>
<xml_diff>
--- a/result/2023_07/mest/2023_07_mest.xlsx
+++ b/result/2023_07/mest/2023_07_mest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="96">
   <si>
     <t>2023_07</t>
   </si>
@@ -220,6 +220,90 @@
   </si>
   <si>
     <t>84957781590</t>
+  </si>
+  <si>
+    <t>4957833732</t>
+  </si>
+  <si>
+    <t>84959933022</t>
+  </si>
+  <si>
+    <t>84959560880</t>
+  </si>
+  <si>
+    <t>84952155215</t>
+  </si>
+  <si>
+    <t>84952311697</t>
+  </si>
+  <si>
+    <t>84959934175</t>
+  </si>
+  <si>
+    <t>84959933229</t>
+  </si>
+  <si>
+    <t>84959935961</t>
+  </si>
+  <si>
+    <t>84956680103</t>
+  </si>
+  <si>
+    <t>84955262030</t>
+  </si>
+  <si>
+    <t>84956680099</t>
+  </si>
+  <si>
+    <t>84955257040</t>
+  </si>
+  <si>
+    <t>84951233071</t>
+  </si>
+  <si>
+    <t>84952217808</t>
+  </si>
+  <si>
+    <t>84951339594</t>
+  </si>
+  <si>
+    <t>84959805980</t>
+  </si>
+  <si>
+    <t>84956680999</t>
+  </si>
+  <si>
+    <t>84959821010</t>
+  </si>
+  <si>
+    <t>84952151654</t>
+  </si>
+  <si>
+    <t>84951518977</t>
+  </si>
+  <si>
+    <t>84954319696</t>
+  </si>
+  <si>
+    <t>84986020604</t>
+  </si>
+  <si>
+    <t>84957758342</t>
+  </si>
+  <si>
+    <t>84957726735</t>
+  </si>
+  <si>
+    <t>84996812841</t>
+  </si>
+  <si>
+    <t>84959673701</t>
+  </si>
+  <si>
+    <t>84958594217</t>
+  </si>
+  <si>
+    <t>84993022429</t>
   </si>
 </sst>
 </file>
@@ -658,18 +742,18 @@
         <v>8</v>
       </c>
       <c r="C7" s="6">
-        <v>173</v>
+        <v>371</v>
       </c>
       <c r="D7" s="2">
         <v>0.7</v>
       </c>
       <c r="E7" s="2">
-        <v>121.1</v>
+        <v>259.7</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="E8" s="1">
-        <v>133.57</v>
+        <v>272.17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -897,7 +981,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D70"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1844,8 +1928,974 @@
       </c>
     </row>
     <row r="70" spans="1:4">
-      <c r="D70" s="1">
-        <v>173</v>
+      <c r="A70" s="7">
+        <v>45126.48476851852</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D70" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="7">
+        <v>45126.50371527778</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D71" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="7">
+        <v>45126.57116898148</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="7">
+        <v>45126.61304398148</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D73" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="7">
+        <v>45127.57454861111</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D74" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="7">
+        <v>45127.58035879629</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D75" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="7">
+        <v>45127.65478009259</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D76" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="7">
+        <v>45127.68164351852</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D77" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="7">
+        <v>45127.68240740741</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="7">
+        <v>45127.68322916667</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D79" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="7">
+        <v>45127.68633101852</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="7">
+        <v>45127.70820601852</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D81" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="7">
+        <v>45128.44475694445</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D82" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="7">
+        <v>45128.44623842592</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D83" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="7">
+        <v>45128.44689814815</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D84" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="7">
+        <v>45128.45520833333</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D85" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="7">
+        <v>45128.4690162037</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D86" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="7">
+        <v>45128.48349537037</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="7">
+        <v>45128.52438657408</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D88" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="7">
+        <v>45128.57600694444</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D89" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="7">
+        <v>45131.38365740741</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D90" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="7">
+        <v>45131.39666666667</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D91" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="7">
+        <v>45131.39732638889</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D92" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="7">
+        <v>45131.39762731481</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D93" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="7">
+        <v>45131.39851851852</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D94" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="7">
+        <v>45131.43131944445</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="7">
+        <v>45131.43217592593</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D96" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="7">
+        <v>45131.44671296296</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D97" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="7">
+        <v>45131.44766203704</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="7">
+        <v>45131.44835648148</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="7">
+        <v>45131.44927083333</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="7">
+        <v>45131.4675462963</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D101" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="7">
+        <v>45131.58650462963</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D102" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="7">
+        <v>45131.59489583333</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D103" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="7">
+        <v>45131.60178240741</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D104" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4">
+      <c r="A105" s="7">
+        <v>45131.61084490741</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D105" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4">
+      <c r="A106" s="7">
+        <v>45131.64585648148</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D106" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="7">
+        <v>45131.65740740741</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D107" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="7">
+        <v>45131.67141203704</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D108" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4">
+      <c r="A109" s="7">
+        <v>45132.384375</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D109" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4">
+      <c r="A110" s="7">
+        <v>45132.40103009259</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D110" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4">
+      <c r="A111" s="7">
+        <v>45132.40734953704</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C111" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D111" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4">
+      <c r="A112" s="7">
+        <v>45132.42634259259</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D112" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4">
+      <c r="A113" s="7">
+        <v>45133.38702546297</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C113" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D113" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4">
+      <c r="A114" s="7">
+        <v>45133.38724537037</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D114" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4">
+      <c r="A115" s="7">
+        <v>45133.41025462963</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C115" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D115" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4">
+      <c r="A116" s="7">
+        <v>45133.42739583334</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C116" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D116" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4">
+      <c r="A117" s="7">
+        <v>45133.58873842593</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C117" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D117" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4">
+      <c r="A118" s="7">
+        <v>45133.71805555555</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C118" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D118" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4">
+      <c r="A119" s="7">
+        <v>45134.41866898148</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D119" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4">
+      <c r="A120" s="7">
+        <v>45134.42373842592</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D120" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4">
+      <c r="A121" s="7">
+        <v>45134.48091435185</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D121" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4">
+      <c r="A122" s="7">
+        <v>45134.53107638889</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D122" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4">
+      <c r="A123" s="7">
+        <v>45134.53886574074</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D123" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4">
+      <c r="A124" s="7">
+        <v>45134.54436342593</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D124" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4">
+      <c r="A125" s="7">
+        <v>45134.54666666667</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D125" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4">
+      <c r="A126" s="7">
+        <v>45134.54900462963</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D126" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4">
+      <c r="A127" s="7">
+        <v>45134.55630787037</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D127" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4">
+      <c r="A128" s="7">
+        <v>45134.57138888889</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D128" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4">
+      <c r="A129" s="7">
+        <v>45135.54636574074</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D129" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4">
+      <c r="A130" s="7">
+        <v>45135.54664351852</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D130" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4">
+      <c r="A131" s="7">
+        <v>45135.54971064815</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D131" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4">
+      <c r="A132" s="7">
+        <v>45135.56893518518</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D132" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4">
+      <c r="A133" s="7">
+        <v>45135.63960648148</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D133" s="2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4">
+      <c r="A134" s="7">
+        <v>45135.67545138889</v>
+      </c>
+      <c r="B134" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C134" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D134" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4">
+      <c r="A135" s="7">
+        <v>45138.4221875</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D135" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4">
+      <c r="A136" s="7">
+        <v>45138.42259259259</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D136" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4">
+      <c r="A137" s="7">
+        <v>45138.42310185185</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D137" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4">
+      <c r="A138" s="7">
+        <v>45138.58421296296</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D138" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4">
+      <c r="D139" s="1">
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>